<commit_message>
updated exploratory_significance_testing to default to comparing current year with previous year
added explanatory notes to README file

added current year data to 'var read across - time series'
</commit_message>
<xml_diff>
--- a/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
+++ b/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2337714\Documents\R\71-ssb-pcos\code\significance_testing\exploratory_analysis\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1251607\Documents\R\pcos-2023\code\significance_testing\exploratory_analysis\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D7EE31-D925-4E7F-8607-C57013E4FFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93FC48-8B0C-40B0-8FCF-6CCE6B87D9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8070" windowWidth="29040" windowHeight="15720" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="var read across " sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="57">
   <si>
     <t>PCOS4</t>
   </si>
@@ -1133,23 +1133,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A829DFF2-EC61-4116-8FF7-0FB7991EF5DC}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
         <v>2009</v>
       </c>
@@ -1180,8 +1180,11 @@
       <c r="J1" s="9">
         <v>2022</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="9">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1212,8 +1215,11 @@
       <c r="J2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1236,8 +1242,11 @@
       <c r="J3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1260,8 +1269,11 @@
       <c r="J4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1284,8 +1296,11 @@
       <c r="J5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1308,8 +1323,11 @@
       <c r="J6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1332,8 +1350,11 @@
       <c r="J7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1354,8 +1375,11 @@
       <c r="J8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1378,8 +1402,11 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1402,8 +1429,11 @@
       <c r="J10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1434,8 +1464,11 @@
       <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1458,8 +1491,11 @@
       <c r="J12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1482,8 +1518,11 @@
       <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1506,8 +1545,11 @@
       <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1530,8 +1572,11 @@
       <c r="J15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1552,8 +1597,11 @@
       <c r="J16" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1576,8 +1624,11 @@
       <c r="J17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1600,8 +1651,11 @@
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1624,8 +1678,11 @@
       <c r="J19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1642,8 +1699,11 @@
       <c r="J20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1660,8 +1720,11 @@
       <c r="J21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1678,8 +1741,11 @@
       <c r="J22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1696,8 +1762,11 @@
       <c r="J23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1714,8 +1783,11 @@
       <c r="J24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1732,8 +1804,11 @@
       <c r="J25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1750,8 +1825,11 @@
       <c r="J26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1768,8 +1846,11 @@
       <c r="J27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1786,8 +1867,11 @@
       <c r="J28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1804,8 +1888,11 @@
       <c r="J29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1822,8 +1909,11 @@
       <c r="J30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1840,8 +1930,11 @@
       <c r="J31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1858,8 +1951,11 @@
       <c r="J32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1876,8 +1972,11 @@
       <c r="J33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1894,8 +1993,11 @@
       <c r="J34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1912,8 +2014,11 @@
       <c r="J35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1930,8 +2035,11 @@
       <c r="J36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1948,8 +2056,11 @@
       <c r="J37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
         <v>43</v>
       </c>
@@ -1974,8 +2085,11 @@
       <c r="J38" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
         <v>46</v>
       </c>
@@ -1998,8 +2112,11 @@
       <c r="J39" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
         <v>49</v>
       </c>
@@ -2024,8 +2141,11 @@
       <c r="J40" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>54</v>
       </c>
@@ -2050,8 +2170,11 @@
       <c r="J41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>54</v>
       </c>
@@ -2076,8 +2199,11 @@
       <c r="J42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C43" s="5" t="s">
         <v>54</v>
       </c>
@@ -2100,6 +2226,9 @@
         <v>55</v>
       </c>
       <c r="J43" t="s">
+        <v>55</v>
+      </c>
+      <c r="K43" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replacing TrustNIAssembly2 with TrustElectedRep2 for current year
</commit_message>
<xml_diff>
--- a/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
+++ b/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1251607\Documents\R\pcos-2023\code\significance_testing\exploratory_analysis\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD93FC48-8B0C-40B0-8FCF-6CCE6B87D9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A0F67-3854-4C3A-B1B9-3DF6B6DFDD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="var read across " sheetId="1" r:id="rId1"/>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,8 +1518,8 @@
       <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>17</v>
+      <c r="K13" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2235,6 +2235,7 @@
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated var read across.xlsx to for 2024 sig tests
</commit_message>
<xml_diff>
--- a/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
+++ b/code/significance_testing/exploratory_analysis/inputs/var read across - time series.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1251607\Documents\R\pcos-2023\code\significance_testing\exploratory_analysis\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2354435\Documents\R\pcos-2024\code\significance_testing\exploratory_analysis\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A0F67-3854-4C3A-B1B9-3DF6B6DFDD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC26CFBD-D29C-4F81-ADAD-7A6B96360C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{369C3F55-ED05-41A1-A5DF-7D9D865E9E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="var read across " sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="57">
   <si>
     <t>PCOS4</t>
   </si>
@@ -1133,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A829DFF2-EC61-4116-8FF7-0FB7991EF5DC}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,10 +1146,10 @@
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9">
         <v>2009</v>
       </c>
@@ -1183,8 +1183,11 @@
       <c r="K1" s="9">
         <v>2023</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1218,8 +1221,11 @@
       <c r="K2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1245,8 +1251,11 @@
       <c r="K3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1272,8 +1281,11 @@
       <c r="K4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1299,8 +1311,11 @@
       <c r="K5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1326,8 +1341,11 @@
       <c r="K6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1353,8 +1371,11 @@
       <c r="K7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1378,8 +1399,11 @@
       <c r="K8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1405,8 +1429,11 @@
       <c r="K9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1432,8 +1459,11 @@
       <c r="K10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1467,8 +1497,11 @@
       <c r="K11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1494,8 +1527,11 @@
       <c r="K12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1521,8 +1557,11 @@
       <c r="K13" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1548,8 +1587,11 @@
       <c r="K14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1575,8 +1617,11 @@
       <c r="K15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1600,8 +1645,11 @@
       <c r="K16" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1627,8 +1675,11 @@
       <c r="K17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1654,8 +1705,11 @@
       <c r="K18" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1681,8 +1735,11 @@
       <c r="K19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1702,8 +1759,11 @@
       <c r="K20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1723,8 +1783,11 @@
       <c r="K21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1744,8 +1807,11 @@
       <c r="K22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1765,8 +1831,11 @@
       <c r="K23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1786,8 +1855,11 @@
       <c r="K24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1807,8 +1879,11 @@
       <c r="K25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1828,8 +1903,11 @@
       <c r="K26" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1849,8 +1927,11 @@
       <c r="K27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1870,8 +1951,11 @@
       <c r="K28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1891,8 +1975,11 @@
       <c r="K29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1912,8 +1999,11 @@
       <c r="K30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1933,8 +2023,11 @@
       <c r="K31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1954,8 +2047,11 @@
       <c r="K32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1975,8 +2071,11 @@
       <c r="K33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1996,8 +2095,11 @@
       <c r="K34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2017,8 +2119,11 @@
       <c r="K35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2038,8 +2143,11 @@
       <c r="K36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2059,8 +2167,11 @@
       <c r="K37" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
         <v>43</v>
       </c>
@@ -2088,8 +2199,11 @@
       <c r="K38" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L38" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
         <v>46</v>
       </c>
@@ -2115,8 +2229,11 @@
       <c r="K39" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
         <v>49</v>
       </c>
@@ -2144,8 +2261,11 @@
       <c r="K40" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>54</v>
       </c>
@@ -2173,8 +2293,11 @@
       <c r="K41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>54</v>
       </c>
@@ -2202,8 +2325,11 @@
       <c r="K42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C43" s="5" t="s">
         <v>54</v>
       </c>
@@ -2229,6 +2355,9 @@
         <v>55</v>
       </c>
       <c r="K43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>